<commit_message>
Updated a root contents file listing different where-to-find documentation, original & new markdown guide versions etc.
</commit_message>
<xml_diff>
--- a/Contents.xlsx
+++ b/Contents.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Contents" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Link</t>
   </si>
   <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
     <t xml:space="preserve">Todo kanban</t>
   </si>
   <si>
@@ -43,19 +46,121 @@
     <t xml:space="preserve">Converted markdown user guide</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/alexkread/rfuserguide/tree/main/New%20version </t>
+    <t xml:space="preserve">https://github.com/alexkread/rfuserguide/tree/main/_User%20guide%20-%20NEW%20-%20markdown%20converted </t>
   </si>
   <si>
     <t xml:space="preserve">Terminology</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/alexkread/rfuserguide/blob/main/Documentation/Terminology%20consistency.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User guide structure</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/alexkread/rfuserguide/tree/main/Documentation/Structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful links</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/alexkread/rfuserguide/blob/main/Documentation/Useful%20links.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Current RF guides, other TA tool guides, external sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/alexkread/rfuserguide/blob/main/Documentation/Scope.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 1, phase 2, out of scope, future considerations</t>
+  </si>
+  <si>
     <t xml:space="preserve">User guide naming options</t>
   </si>
   <si>
-    <t xml:space="preserve">User guide structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Useful links</t>
+    <t xml:space="preserve">https://github.com/alexkread/rfuserguide/blob/main/Documentation/User%20guide%20naming%20options.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation types found throughout RF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/alexkread/rfuserguide/blob/main/Documentation/Documentation%20types%20found%20throughout%20RF.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -65,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,8 +200,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="6"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -157,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +289,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,16 +483,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="78.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="63.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,56 +503,99 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://alexkreadrf.kanbantool.com/b/1084109"/>
     <hyperlink ref="B3" r:id="rId2" display="https://robotframework.org/robotframework/latest/RobotFrameworkUserGuide.html"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/alexkread/rfuserguide/tree/main/New%20version "/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/alexkread/rfuserguide/tree/main/_User%20guide%20-%20NEW%20-%20markdown%20converted"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/alexkread/rfuserguide/blob/main/Documentation/Terminology%20consistency.xlsx"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/alexkread/rfuserguide/tree/main/Documentation/Structure"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/alexkread/rfuserguide/blob/main/Documentation/Useful%20links.xlsx"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://github.com/alexkread/rfuserguide/blob/main/Documentation/Scope.xlsx"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://github.com/alexkread/rfuserguide/blob/main/Documentation/User%20guide%20naming%20options.txt"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://github.com/alexkread/rfuserguide/blob/main/Documentation/Documentation%20types%20found%20throughout%20RF.txt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>